<commit_message>
get fear and greed everyday
</commit_message>
<xml_diff>
--- a/data/README_data_common.xlsx
+++ b/data/README_data_common.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ipynb\factors_affecting_stock_price\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A775B07-2701-4D37-824E-168FD626D3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32535" yWindow="3420" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32535" yWindow="3420" windowWidth="20025" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
@@ -753,8 +752,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -782,6 +781,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -803,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -811,6 +825,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1090,11 +1108,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1162,7 +1180,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C3" t="s">
@@ -1199,7 +1217,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C5" t="s">
@@ -1227,7 +1245,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C7" t="s">
@@ -1255,7 +1273,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C9" t="s">
@@ -1283,7 +1301,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>110</v>
       </c>
       <c r="C11" t="s">
@@ -1311,7 +1329,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C13" t="s">
@@ -1339,7 +1357,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C15" t="s">
@@ -1367,7 +1385,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C17" t="s">
@@ -1395,7 +1413,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C19" t="s">
@@ -1423,7 +1441,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C21" t="s">
@@ -1451,7 +1469,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C23" t="s">
@@ -1479,7 +1497,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C25" t="s">
@@ -1507,7 +1525,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C27" t="s">
@@ -1535,7 +1553,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C29" t="s">
@@ -1563,7 +1581,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C31" t="s">
@@ -1591,7 +1609,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C33" t="s">
@@ -1619,7 +1637,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C35" t="s">
@@ -1661,7 +1679,7 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C38" t="s">
@@ -1689,7 +1707,7 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1703,7 +1721,7 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C41" t="s">
@@ -1717,7 +1735,7 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="6" t="s">
         <v>116</v>
       </c>
       <c r="C42" t="s">

</xml_diff>

<commit_message>
add logic for fed rate and bok rate
</commit_message>
<xml_diff>
--- a/data/README_data_common.xlsx
+++ b/data/README_data_common.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ipynb\factors_affecting_stock_price\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F824648-FC66-41B0-8C96-C65A2CACD4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32535" yWindow="3420" windowWidth="20025" windowHeight="12030"/>
+    <workbookView xWindow="29655" yWindow="2550" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -752,7 +761,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -826,9 +835,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1108,11 +1119,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1208,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C4" t="s">
@@ -1231,7 +1242,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C6" t="s">
@@ -1259,7 +1270,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C8" t="s">
@@ -1287,7 +1298,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C10" t="s">
@@ -1315,7 +1326,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C12" t="s">
@@ -1343,7 +1354,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C14" t="s">
@@ -1371,7 +1382,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C16" t="s">
@@ -1399,7 +1410,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C18" t="s">
@@ -1427,7 +1438,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C20" t="s">
@@ -1455,7 +1466,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C22" t="s">
@@ -1483,7 +1494,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>132</v>
       </c>
       <c r="C24" t="s">
@@ -1511,7 +1522,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>135</v>
       </c>
       <c r="C26" t="s">
@@ -1539,7 +1550,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>138</v>
       </c>
       <c r="C28" t="s">
@@ -1553,7 +1564,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C29" t="s">
@@ -1567,7 +1578,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C30" t="s">
@@ -1581,7 +1592,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C31" t="s">
@@ -1595,7 +1606,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>140</v>
       </c>
       <c r="C32" t="s">
@@ -1609,7 +1620,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C33" t="s">
@@ -1623,7 +1634,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>141</v>
       </c>
       <c r="C34" t="s">
@@ -1651,7 +1662,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C36" t="s">
@@ -1665,7 +1676,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C37" t="s">
@@ -1693,7 +1704,7 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1721,7 +1732,7 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C41" t="s">
@@ -1735,7 +1746,7 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C42" t="s">
@@ -1749,7 +1760,7 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C43" t="s">
@@ -1763,7 +1774,7 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C44" t="s">

</xml_diff>